<commit_message>
fix: fix sample statement file
</commit_message>
<xml_diff>
--- a/samples/statements-sample.xlsx
+++ b/samples/statements-sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VAID\DATA\IMPORTANT\FINANCIAL\FINSUM\per-fin-dash\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ADE19F-5491-424C-8542-D8305A42C11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB39ACD-6FDD-4DD6-A3B8-6E9C6DFF9560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="statements" sheetId="1" r:id="rId1"/>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD6C0A4-5F47-4F91-B85C-2425C33893D0}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1531,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6360CE86-9208-42ED-AA7F-12467A23FD69}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1746,7 +1746,7 @@
       <c r="F10" t="s">
         <v>33</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>35000</v>
       </c>
       <c r="J10" t="s">

</xml_diff>